<commit_message>
update fri 2/23 2pm
</commit_message>
<xml_diff>
--- a/results/tables_MHT_analysis.xlsx
+++ b/results/tables_MHT_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1140" windowWidth="27300" windowHeight="17900" tabRatio="822" activeTab="3"/>
+    <workbookView xWindow="1000" yWindow="1140" windowWidth="27300" windowHeight="17900" tabRatio="822" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - Hypertension Status" sheetId="3" r:id="rId1"/>
@@ -931,7 +931,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1072,6 +1072,9 @@
     <xf numFmtId="11" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2760,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2985,7 +2988,7 @@
       <c r="D11" s="61">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="90">
         <v>4.7544096626499999E-2</v>
       </c>
       <c r="F11" s="38">
@@ -3010,7 +3013,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3493,8 +3496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>